<commit_message>
feat: change export button position
</commit_message>
<xml_diff>
--- a/public/business-conf.xlsx
+++ b/public/business-conf.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="596">
   <si>
     <t>id</t>
   </si>
@@ -64,6 +64,9 @@
     <t>registerType</t>
   </si>
   <si>
+    <t>city</t>
+  </si>
+  <si>
     <t>Михаил</t>
   </si>
   <si>
@@ -1007,6 +1010,795 @@
   </si>
   <si>
     <t>2025-05-19T04:14:09.494Z</t>
+  </si>
+  <si>
+    <t>Маис</t>
+  </si>
+  <si>
+    <t>Айвазян</t>
+  </si>
+  <si>
+    <t>Геворгович</t>
+  </si>
+  <si>
+    <t>89150753519</t>
+  </si>
+  <si>
+    <t>mayis.ayvazyan@yandex.ru</t>
+  </si>
+  <si>
+    <t>Финансы, бухгалтерия</t>
+  </si>
+  <si>
+    <t>197327</t>
+  </si>
+  <si>
+    <t>2025-05-21T11:26:23.645Z</t>
+  </si>
+  <si>
+    <t>2025-05-21T11:27:57.707Z</t>
+  </si>
+  <si>
+    <t>2025-05-21T11:26:23.580Z</t>
+  </si>
+  <si>
+    <t>Игорь</t>
+  </si>
+  <si>
+    <t>Романов</t>
+  </si>
+  <si>
+    <t>+79518107456</t>
+  </si>
+  <si>
+    <t>gs-potolok@mail.ru</t>
+  </si>
+  <si>
+    <t>Религиозная группа "Дом Отца"</t>
+  </si>
+  <si>
+    <t>420610</t>
+  </si>
+  <si>
+    <t>2025-05-24T11:30:55.580Z</t>
+  </si>
+  <si>
+    <t>2025-05-24T11:31:53.108Z</t>
+  </si>
+  <si>
+    <t>2025-05-24T11:30:55.502Z</t>
+  </si>
+  <si>
+    <t>Егор</t>
+  </si>
+  <si>
+    <t>Вечерский</t>
+  </si>
+  <si>
+    <t>Александрович</t>
+  </si>
+  <si>
+    <t>+79028617427</t>
+  </si>
+  <si>
+    <t>egor@teh-u.ru</t>
+  </si>
+  <si>
+    <t>Новая жизнь</t>
+  </si>
+  <si>
+    <t>190463</t>
+  </si>
+  <si>
+    <t>2025-05-28T12:40:15.881Z</t>
+  </si>
+  <si>
+    <t>2025-05-28T12:41:03.425Z</t>
+  </si>
+  <si>
+    <t>2025-05-28T12:40:15.858Z</t>
+  </si>
+  <si>
+    <t>Челябинск</t>
+  </si>
+  <si>
+    <t>Ирина</t>
+  </si>
+  <si>
+    <t>Русалеева</t>
+  </si>
+  <si>
+    <t>89043023676</t>
+  </si>
+  <si>
+    <t>malshkola@yandex.ru</t>
+  </si>
+  <si>
+    <t>образование детей</t>
+  </si>
+  <si>
+    <t>979309</t>
+  </si>
+  <si>
+    <t>2025-05-28T13:19:28.651Z</t>
+  </si>
+  <si>
+    <t>2025-05-28T13:22:48.205Z</t>
+  </si>
+  <si>
+    <t>2025-05-28T13:19:28.637Z</t>
+  </si>
+  <si>
+    <t>Виктория</t>
+  </si>
+  <si>
+    <t>Топоркова</t>
+  </si>
+  <si>
+    <t>Семеновна</t>
+  </si>
+  <si>
+    <t>89631556041</t>
+  </si>
+  <si>
+    <t>viktoriatoporkova@mail.ru</t>
+  </si>
+  <si>
+    <t>542827</t>
+  </si>
+  <si>
+    <t>2025-05-28T14:08:48.549Z</t>
+  </si>
+  <si>
+    <t>2025-05-28T14:12:15.256Z</t>
+  </si>
+  <si>
+    <t>2025-05-28T14:08:48.539Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Челябинск </t>
+  </si>
+  <si>
+    <t>Сергей</t>
+  </si>
+  <si>
+    <t>Ищенко</t>
+  </si>
+  <si>
+    <t>8 705 658 46 80</t>
+  </si>
+  <si>
+    <t>homepremier@mail.ru</t>
+  </si>
+  <si>
+    <t>Христианский Семейный Центр</t>
+  </si>
+  <si>
+    <t>Сдача в аренду недвижимости</t>
+  </si>
+  <si>
+    <t>333102</t>
+  </si>
+  <si>
+    <t>2025-05-29T03:19:56.024Z</t>
+  </si>
+  <si>
+    <t>2025-05-29T03:37:55.005Z</t>
+  </si>
+  <si>
+    <t>2025-05-29T03:19:55.904Z</t>
+  </si>
+  <si>
+    <t>Житикара</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Анатолий </t>
+  </si>
+  <si>
+    <t>Дубинин</t>
+  </si>
+  <si>
+    <t>+7 905 845 0066</t>
+  </si>
+  <si>
+    <t>kris811@mail.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Благая весть </t>
+  </si>
+  <si>
+    <t>136997</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:33:49.771Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:51:16.576Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:33:49.642Z</t>
+  </si>
+  <si>
+    <t>Орск</t>
+  </si>
+  <si>
+    <t>Светлана</t>
+  </si>
+  <si>
+    <t>Дубинина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Анатольевна </t>
+  </si>
+  <si>
+    <t>+7 905 847 9080</t>
+  </si>
+  <si>
+    <t>210324</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:52:46.094Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:53:15.235Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:52:46.086Z</t>
+  </si>
+  <si>
+    <t>Евгений</t>
+  </si>
+  <si>
+    <t>Шиповалов</t>
+  </si>
+  <si>
+    <t>89376341415</t>
+  </si>
+  <si>
+    <t>almi.evgen@mail.ru</t>
+  </si>
+  <si>
+    <t>83874</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:58:16.527Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:59:22.996Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T07:58:16.520Z</t>
+  </si>
+  <si>
+    <t>Яков</t>
+  </si>
+  <si>
+    <t>Попов</t>
+  </si>
+  <si>
+    <t>Алексеевич</t>
+  </si>
+  <si>
+    <t>+7 (919) 116-03-51</t>
+  </si>
+  <si>
+    <t>Uralprom14@mail.ru</t>
+  </si>
+  <si>
+    <t>Продажи</t>
+  </si>
+  <si>
+    <t>699945</t>
+  </si>
+  <si>
+    <t>2025-05-30T09:09:11.317Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T09:11:49.539Z</t>
+  </si>
+  <si>
+    <t>2025-05-30T09:09:11.254Z</t>
+  </si>
+  <si>
+    <t>Владимир</t>
+  </si>
+  <si>
+    <t>Катьянов</t>
+  </si>
+  <si>
+    <t>Сергеевич</t>
+  </si>
+  <si>
+    <t>89678737763</t>
+  </si>
+  <si>
+    <t>katyanov.vs@yandex.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гора Сион </t>
+  </si>
+  <si>
+    <t>237291</t>
+  </si>
+  <si>
+    <t>2025-05-31T05:03:58.355Z</t>
+  </si>
+  <si>
+    <t>2025-05-31T05:56:30.437Z</t>
+  </si>
+  <si>
+    <t>2025-05-31T05:03:58.342Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Екатеринбург </t>
+  </si>
+  <si>
+    <t>Мария</t>
+  </si>
+  <si>
+    <t>Куцак</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Викторовна </t>
+  </si>
+  <si>
+    <t>89000793791</t>
+  </si>
+  <si>
+    <t>zolushka.174@mail.ru</t>
+  </si>
+  <si>
+    <t>Краеугольный камень</t>
+  </si>
+  <si>
+    <t>278001</t>
+  </si>
+  <si>
+    <t>2025-05-31T12:06:29.415Z</t>
+  </si>
+  <si>
+    <t>2025-05-31T12:08:15.014Z</t>
+  </si>
+  <si>
+    <t>2025-05-31T12:06:29.409Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сергей </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мартюничев </t>
+  </si>
+  <si>
+    <t>Викторович</t>
+  </si>
+  <si>
+    <t>+79252236561</t>
+  </si>
+  <si>
+    <t>vozhak77@me.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Словно жизни </t>
+  </si>
+  <si>
+    <t>853621</t>
+  </si>
+  <si>
+    <t>2025-05-31T18:10:31.715Z</t>
+  </si>
+  <si>
+    <t>2025-05-31T18:11:30.996Z</t>
+  </si>
+  <si>
+    <t>2025-05-31T18:10:31.667Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Москва </t>
+  </si>
+  <si>
+    <t>Иван</t>
+  </si>
+  <si>
+    <t>Мальцев</t>
+  </si>
+  <si>
+    <t>Вадимович</t>
+  </si>
+  <si>
+    <t>89174506473</t>
+  </si>
+  <si>
+    <t>maltcev_ivan@bk.ru</t>
+  </si>
+  <si>
+    <t>Христа Спасителя</t>
+  </si>
+  <si>
+    <t>214069</t>
+  </si>
+  <si>
+    <t>2025-06-01T05:42:47.700Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T05:44:10.037Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T05:42:47.612Z</t>
+  </si>
+  <si>
+    <t>Уфа</t>
+  </si>
+  <si>
+    <t>Виктор</t>
+  </si>
+  <si>
+    <t>Кузьминых</t>
+  </si>
+  <si>
+    <t>+79127700012</t>
+  </si>
+  <si>
+    <t>kuzminyhvn@mail.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Строительство </t>
+  </si>
+  <si>
+    <t>904999</t>
+  </si>
+  <si>
+    <t>2025-06-01T05:43:58.627Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T05:53:25.562Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T05:43:58.617Z</t>
+  </si>
+  <si>
+    <t>Ольга</t>
+  </si>
+  <si>
+    <t>Выползова</t>
+  </si>
+  <si>
+    <t>89090762695</t>
+  </si>
+  <si>
+    <t>lizapol@yandex.ru</t>
+  </si>
+  <si>
+    <t>Слово жизни Челябинск</t>
+  </si>
+  <si>
+    <t>розничная торговля</t>
+  </si>
+  <si>
+    <t>37511</t>
+  </si>
+  <si>
+    <t>2025-06-01T11:55:23.557Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T11:56:18.126Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T11:55:23.461Z</t>
+  </si>
+  <si>
+    <t>Копейск</t>
+  </si>
+  <si>
+    <t>Николай</t>
+  </si>
+  <si>
+    <t>Буртыненко</t>
+  </si>
+  <si>
+    <t>9080804993</t>
+  </si>
+  <si>
+    <t>ask.gidro2@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Промышленный клининг </t>
+  </si>
+  <si>
+    <t>662089</t>
+  </si>
+  <si>
+    <t>2025-06-01T12:04:51.498Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T12:06:58.565Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T12:04:51.390Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Екатерина </t>
+  </si>
+  <si>
+    <t>Рисованая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Олеговна </t>
+  </si>
+  <si>
+    <t>risovaniy@icloud.com</t>
+  </si>
+  <si>
+    <t>Бьюти</t>
+  </si>
+  <si>
+    <t>54764</t>
+  </si>
+  <si>
+    <t>2025-06-01T12:14:54.868Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T12:16:16.570Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T12:14:54.792Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лидия </t>
+  </si>
+  <si>
+    <t>Комарских</t>
+  </si>
+  <si>
+    <t>+7 993 934 0993</t>
+  </si>
+  <si>
+    <t>lidochka21@vk.com</t>
+  </si>
+  <si>
+    <t>учусь</t>
+  </si>
+  <si>
+    <t>680752</t>
+  </si>
+  <si>
+    <t>2025-06-01T13:44:06.867Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T13:44:53.175Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T13:44:06.859Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Малышева </t>
+  </si>
+  <si>
+    <t>89630885957</t>
+  </si>
+  <si>
+    <t>ya.love.e@yandex.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Недвижимость </t>
+  </si>
+  <si>
+    <t>631368</t>
+  </si>
+  <si>
+    <t>2025-06-01T16:11:07.674Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T16:12:33.026Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T16:11:07.621Z</t>
+  </si>
+  <si>
+    <t>Вишнякова</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Николаевна </t>
+  </si>
+  <si>
+    <t>89823657463</t>
+  </si>
+  <si>
+    <t>svolkova174@gmail.com</t>
+  </si>
+  <si>
+    <t>Питание</t>
+  </si>
+  <si>
+    <t>270360</t>
+  </si>
+  <si>
+    <t>2025-06-01T17:56:24.791Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T17:57:35.181Z</t>
+  </si>
+  <si>
+    <t>2025-06-01T17:56:24.787Z</t>
+  </si>
+  <si>
+    <t>Андрей</t>
+  </si>
+  <si>
+    <t>Филиппов</t>
+  </si>
+  <si>
+    <t>Дмитриевич</t>
+  </si>
+  <si>
+    <t>+7 9085823123</t>
+  </si>
+  <si>
+    <t>seriousandre@gmail.com</t>
+  </si>
+  <si>
+    <t>Слово Жизни Челябинск</t>
+  </si>
+  <si>
+    <t>Медиа</t>
+  </si>
+  <si>
+    <t>144034</t>
+  </si>
+  <si>
+    <t>2025-06-02T19:07:55.044Z</t>
+  </si>
+  <si>
+    <t>2025-06-02T19:08:55.334Z</t>
+  </si>
+  <si>
+    <t>2025-06-02T19:07:55.035Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Марина </t>
+  </si>
+  <si>
+    <t>Валькова</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Юрьевна </t>
+  </si>
+  <si>
+    <t>89822930182</t>
+  </si>
+  <si>
+    <t>cdrsol@mail.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Свет миру </t>
+  </si>
+  <si>
+    <t>Прихожане</t>
+  </si>
+  <si>
+    <t>736052</t>
+  </si>
+  <si>
+    <t>2025-06-04T05:27:26.368Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T05:28:24.049Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T05:27:26.328Z</t>
+  </si>
+  <si>
+    <t>Арсений</t>
+  </si>
+  <si>
+    <t>Хворонов</t>
+  </si>
+  <si>
+    <t>Анатольевич</t>
+  </si>
+  <si>
+    <t>89630762556</t>
+  </si>
+  <si>
+    <t>doit-01@mail.ru</t>
+  </si>
+  <si>
+    <t>Гора Сион</t>
+  </si>
+  <si>
+    <t>христианин</t>
+  </si>
+  <si>
+    <t>348445</t>
+  </si>
+  <si>
+    <t>2025-06-04T07:15:57.068Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T07:17:32.902Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T07:15:57.062Z</t>
+  </si>
+  <si>
+    <t>Екатеринбург</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гребенников </t>
+  </si>
+  <si>
+    <t>89667707561</t>
+  </si>
+  <si>
+    <t>market_victory@mail.ru</t>
+  </si>
+  <si>
+    <t>241464</t>
+  </si>
+  <si>
+    <t>2025-06-04T07:58:39.804Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T07:59:36.073Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T07:58:39.736Z</t>
+  </si>
+  <si>
+    <t>Кузин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тимофеевич </t>
+  </si>
+  <si>
+    <t>+79506960728</t>
+  </si>
+  <si>
+    <t>mkuzin72@yandex.ru</t>
+  </si>
+  <si>
+    <t>ЕХБ "Надежда"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Автозапчасти </t>
+  </si>
+  <si>
+    <t>176904</t>
+  </si>
+  <si>
+    <t>2025-06-04T18:52:56.327Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T18:53:31.004Z</t>
+  </si>
+  <si>
+    <t>2025-06-04T18:52:56.321Z</t>
+  </si>
+  <si>
+    <t>Дятьково</t>
+  </si>
+  <si>
+    <t>Окунев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вячеславович </t>
+  </si>
+  <si>
+    <t>89227494477</t>
+  </si>
+  <si>
+    <t>okunishka@mail.ru</t>
+  </si>
+  <si>
+    <t>895964</t>
+  </si>
+  <si>
+    <t>2025-06-06T09:48:15.487Z</t>
+  </si>
+  <si>
+    <t>2025-06-06T09:49:11.033Z</t>
+  </si>
+  <si>
+    <t>2025-06-06T09:48:15.432Z</t>
   </si>
 </sst>
 </file>
@@ -1383,13 +2175,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:R59"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="17" width="20" customWidth="1"/>
+    <col min="1" max="18" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1441,1468 +2233,2743 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="P6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O8" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="P9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="P10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="N11" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="O11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="P11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="P12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="N13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="O13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="P13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="P14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="O15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C16" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="O16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="P16" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F17" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="P17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C18" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="N19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="O19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="P19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E20" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M20" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N20" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O20" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C21" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G21" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M21" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="N21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O21" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="P21" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C22" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D22" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E22" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J22" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M22" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N22" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="O22" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="P22" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C23" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D23" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F23" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G23" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J23" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="K23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M23" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N23" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O23" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="P23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C24" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D24" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F24" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G24" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J24" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="K24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M24" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N24" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="O24" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="P24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E25" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F25" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G25" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M25" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N25" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O25" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P25" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D26" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E26" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F26" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G26" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M26" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="N26" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="O26" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P26" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C27" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F27" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G27" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="I27" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K27" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M27" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="N27" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="O27" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="P27" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C28" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D28" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E28" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F28" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="G28" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J28" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="K28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M28" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N28" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="O28" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="P28" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C29" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D29" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E29" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F29" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G29" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I29" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="J29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M29" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N29" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="O29" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="P29" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D30" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E30" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F30" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G30" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I30" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="J30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M30" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N30" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="O30" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="P30" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C31" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D31" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="E31" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F31" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G31" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M31" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N31" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="O31" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="P31" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C32" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E32" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F32" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G32" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J32" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="K32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" t="s">
+        <v>329</v>
+      </c>
+      <c r="N32" t="s">
+        <v>330</v>
+      </c>
+      <c r="O32" t="s">
+        <v>331</v>
+      </c>
+      <c r="P32" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>333</v>
+      </c>
+      <c r="C33" t="s">
+        <v>334</v>
+      </c>
+      <c r="D33" t="s">
+        <v>335</v>
+      </c>
+      <c r="E33" t="s">
+        <v>336</v>
+      </c>
+      <c r="F33" t="s">
+        <v>337</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" t="s">
+        <v>338</v>
+      </c>
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" t="s">
+        <v>339</v>
+      </c>
+      <c r="N33" t="s">
+        <v>340</v>
+      </c>
+      <c r="O33" t="s">
+        <v>341</v>
+      </c>
+      <c r="P33" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C34" t="s">
+        <v>344</v>
+      </c>
+      <c r="D34" t="s">
+        <v>316</v>
+      </c>
+      <c r="E34" t="s">
+        <v>345</v>
+      </c>
+      <c r="F34" t="s">
+        <v>346</v>
+      </c>
+      <c r="G34" t="s">
+        <v>347</v>
+      </c>
+      <c r="J34" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" t="s">
+        <v>71</v>
+      </c>
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" t="s">
+        <v>348</v>
+      </c>
+      <c r="N34" t="s">
+        <v>349</v>
+      </c>
+      <c r="O34" t="s">
+        <v>350</v>
+      </c>
+      <c r="P34" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>352</v>
+      </c>
+      <c r="C35" t="s">
+        <v>353</v>
+      </c>
+      <c r="D35" t="s">
+        <v>354</v>
+      </c>
+      <c r="E35" t="s">
+        <v>355</v>
+      </c>
+      <c r="F35" t="s">
+        <v>356</v>
+      </c>
+      <c r="G35" t="s">
+        <v>357</v>
+      </c>
+      <c r="J35" t="s">
         <v>25</v>
       </c>
-      <c r="L32" t="s">
+      <c r="K35" t="s">
         <v>26</v>
       </c>
-      <c r="M32" t="s">
-        <v>328</v>
-      </c>
-      <c r="N32" t="s">
-        <v>329</v>
-      </c>
-      <c r="O32" t="s">
-        <v>330</v>
-      </c>
-      <c r="P32" t="s">
-        <v>331</v>
+      <c r="L35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" t="s">
+        <v>358</v>
+      </c>
+      <c r="N35" t="s">
+        <v>359</v>
+      </c>
+      <c r="O35" t="s">
+        <v>360</v>
+      </c>
+      <c r="P35" t="s">
+        <v>361</v>
+      </c>
+      <c r="R35" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>363</v>
+      </c>
+      <c r="C36" t="s">
+        <v>364</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" t="s">
+        <v>365</v>
+      </c>
+      <c r="F36" t="s">
+        <v>366</v>
+      </c>
+      <c r="G36" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" t="s">
+        <v>367</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>368</v>
+      </c>
+      <c r="N36" t="s">
+        <v>369</v>
+      </c>
+      <c r="O36" t="s">
+        <v>370</v>
+      </c>
+      <c r="P36" t="s">
+        <v>371</v>
+      </c>
+      <c r="R36" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>372</v>
+      </c>
+      <c r="C37" t="s">
+        <v>373</v>
+      </c>
+      <c r="D37" t="s">
+        <v>374</v>
+      </c>
+      <c r="E37" t="s">
+        <v>375</v>
+      </c>
+      <c r="F37" t="s">
+        <v>376</v>
+      </c>
+      <c r="G37" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" t="s">
+        <v>131</v>
+      </c>
+      <c r="J37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K37" t="s">
+        <v>132</v>
+      </c>
+      <c r="L37" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37" t="s">
+        <v>377</v>
+      </c>
+      <c r="N37" t="s">
+        <v>378</v>
+      </c>
+      <c r="O37" t="s">
+        <v>379</v>
+      </c>
+      <c r="P37" t="s">
+        <v>380</v>
+      </c>
+      <c r="R37" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>382</v>
+      </c>
+      <c r="C38" t="s">
+        <v>383</v>
+      </c>
+      <c r="D38" t="s">
+        <v>354</v>
+      </c>
+      <c r="E38" t="s">
+        <v>384</v>
+      </c>
+      <c r="F38" t="s">
+        <v>385</v>
+      </c>
+      <c r="G38" t="s">
+        <v>386</v>
+      </c>
+      <c r="J38" t="s">
+        <v>387</v>
+      </c>
+      <c r="K38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" t="s">
+        <v>27</v>
+      </c>
+      <c r="M38" t="s">
+        <v>388</v>
+      </c>
+      <c r="N38" t="s">
+        <v>389</v>
+      </c>
+      <c r="O38" t="s">
+        <v>390</v>
+      </c>
+      <c r="P38" t="s">
+        <v>391</v>
+      </c>
+      <c r="R38" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>110</v>
+      </c>
+      <c r="B39" t="s">
+        <v>393</v>
+      </c>
+      <c r="C39" t="s">
+        <v>394</v>
+      </c>
+      <c r="D39" t="s">
+        <v>354</v>
+      </c>
+      <c r="E39" t="s">
+        <v>395</v>
+      </c>
+      <c r="F39" t="s">
+        <v>396</v>
+      </c>
+      <c r="G39" t="s">
+        <v>397</v>
+      </c>
+      <c r="J39" t="s">
+        <v>219</v>
+      </c>
+      <c r="K39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>27</v>
+      </c>
+      <c r="M39" t="s">
+        <v>398</v>
+      </c>
+      <c r="N39" t="s">
+        <v>399</v>
+      </c>
+      <c r="O39" t="s">
+        <v>400</v>
+      </c>
+      <c r="P39" t="s">
+        <v>401</v>
+      </c>
+      <c r="R39" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>111</v>
+      </c>
+      <c r="B40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C40" t="s">
+        <v>404</v>
+      </c>
+      <c r="D40" t="s">
+        <v>405</v>
+      </c>
+      <c r="E40" t="s">
+        <v>406</v>
+      </c>
+      <c r="F40" t="s">
+        <v>396</v>
+      </c>
+      <c r="G40" t="s">
+        <v>397</v>
+      </c>
+      <c r="J40" t="s">
+        <v>219</v>
+      </c>
+      <c r="K40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40" t="s">
+        <v>27</v>
+      </c>
+      <c r="M40" t="s">
+        <v>407</v>
+      </c>
+      <c r="N40" t="s">
+        <v>408</v>
+      </c>
+      <c r="O40" t="s">
+        <v>409</v>
+      </c>
+      <c r="P40" t="s">
+        <v>410</v>
+      </c>
+      <c r="R40" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>112</v>
+      </c>
+      <c r="B41" t="s">
+        <v>411</v>
+      </c>
+      <c r="C41" t="s">
+        <v>412</v>
+      </c>
+      <c r="D41" t="s">
+        <v>354</v>
+      </c>
+      <c r="E41" t="s">
+        <v>413</v>
+      </c>
+      <c r="F41" t="s">
+        <v>414</v>
+      </c>
+      <c r="G41" t="s">
+        <v>48</v>
+      </c>
+      <c r="J41" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" t="s">
+        <v>71</v>
+      </c>
+      <c r="L41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M41" t="s">
+        <v>415</v>
+      </c>
+      <c r="N41" t="s">
+        <v>416</v>
+      </c>
+      <c r="O41" t="s">
+        <v>417</v>
+      </c>
+      <c r="P41" t="s">
+        <v>418</v>
+      </c>
+      <c r="R41" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>113</v>
+      </c>
+      <c r="B42" t="s">
+        <v>419</v>
+      </c>
+      <c r="C42" t="s">
+        <v>420</v>
+      </c>
+      <c r="D42" t="s">
+        <v>421</v>
+      </c>
+      <c r="E42" t="s">
+        <v>422</v>
+      </c>
+      <c r="F42" t="s">
+        <v>423</v>
+      </c>
+      <c r="G42" t="s">
+        <v>218</v>
+      </c>
+      <c r="J42" t="s">
+        <v>424</v>
+      </c>
+      <c r="K42" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" t="s">
+        <v>27</v>
+      </c>
+      <c r="M42" t="s">
+        <v>425</v>
+      </c>
+      <c r="N42" t="s">
+        <v>426</v>
+      </c>
+      <c r="O42" t="s">
+        <v>427</v>
+      </c>
+      <c r="P42" t="s">
+        <v>428</v>
+      </c>
+      <c r="R42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>429</v>
+      </c>
+      <c r="C43" t="s">
+        <v>430</v>
+      </c>
+      <c r="D43" t="s">
+        <v>431</v>
+      </c>
+      <c r="E43" t="s">
+        <v>432</v>
+      </c>
+      <c r="F43" t="s">
+        <v>433</v>
+      </c>
+      <c r="G43" t="s">
+        <v>434</v>
+      </c>
+      <c r="J43" t="s">
+        <v>24</v>
+      </c>
+      <c r="K43" t="s">
+        <v>71</v>
+      </c>
+      <c r="L43" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43" t="s">
+        <v>435</v>
+      </c>
+      <c r="N43" t="s">
+        <v>436</v>
+      </c>
+      <c r="O43" t="s">
+        <v>437</v>
+      </c>
+      <c r="P43" t="s">
+        <v>438</v>
+      </c>
+      <c r="R43" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>440</v>
+      </c>
+      <c r="C44" t="s">
+        <v>441</v>
+      </c>
+      <c r="D44" t="s">
+        <v>442</v>
+      </c>
+      <c r="E44" t="s">
+        <v>443</v>
+      </c>
+      <c r="F44" t="s">
+        <v>444</v>
+      </c>
+      <c r="G44" t="s">
+        <v>445</v>
+      </c>
+      <c r="J44" t="s">
+        <v>198</v>
+      </c>
+      <c r="K44" t="s">
+        <v>26</v>
+      </c>
+      <c r="L44" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44" t="s">
+        <v>446</v>
+      </c>
+      <c r="N44" t="s">
+        <v>447</v>
+      </c>
+      <c r="O44" t="s">
+        <v>448</v>
+      </c>
+      <c r="P44" t="s">
+        <v>449</v>
+      </c>
+      <c r="R44" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>119</v>
+      </c>
+      <c r="B45" t="s">
+        <v>450</v>
+      </c>
+      <c r="C45" t="s">
+        <v>451</v>
+      </c>
+      <c r="D45" t="s">
+        <v>452</v>
+      </c>
+      <c r="E45" t="s">
+        <v>453</v>
+      </c>
+      <c r="F45" t="s">
+        <v>454</v>
+      </c>
+      <c r="G45" t="s">
+        <v>455</v>
+      </c>
+      <c r="J45" t="s">
+        <v>24</v>
+      </c>
+      <c r="K45" t="s">
+        <v>71</v>
+      </c>
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" t="s">
+        <v>456</v>
+      </c>
+      <c r="N45" t="s">
+        <v>457</v>
+      </c>
+      <c r="O45" t="s">
+        <v>458</v>
+      </c>
+      <c r="P45" t="s">
+        <v>459</v>
+      </c>
+      <c r="R45" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>121</v>
+      </c>
+      <c r="B46" t="s">
+        <v>461</v>
+      </c>
+      <c r="C46" t="s">
+        <v>462</v>
+      </c>
+      <c r="D46" t="s">
+        <v>463</v>
+      </c>
+      <c r="E46" t="s">
+        <v>464</v>
+      </c>
+      <c r="F46" t="s">
+        <v>465</v>
+      </c>
+      <c r="G46" t="s">
+        <v>466</v>
+      </c>
+      <c r="J46" t="s">
+        <v>24</v>
+      </c>
+      <c r="K46" t="s">
+        <v>71</v>
+      </c>
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" t="s">
+        <v>467</v>
+      </c>
+      <c r="N46" t="s">
+        <v>468</v>
+      </c>
+      <c r="O46" t="s">
+        <v>469</v>
+      </c>
+      <c r="P46" t="s">
+        <v>470</v>
+      </c>
+      <c r="R46" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>122</v>
+      </c>
+      <c r="B47" t="s">
+        <v>472</v>
+      </c>
+      <c r="C47" t="s">
+        <v>473</v>
+      </c>
+      <c r="D47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" t="s">
+        <v>474</v>
+      </c>
+      <c r="F47" t="s">
+        <v>475</v>
+      </c>
+      <c r="G47" t="s">
+        <v>69</v>
+      </c>
+      <c r="J47" t="s">
+        <v>476</v>
+      </c>
+      <c r="K47" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" t="s">
+        <v>477</v>
+      </c>
+      <c r="N47" t="s">
+        <v>478</v>
+      </c>
+      <c r="O47" t="s">
+        <v>479</v>
+      </c>
+      <c r="P47" t="s">
+        <v>480</v>
+      </c>
+      <c r="R47" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>123</v>
+      </c>
+      <c r="B48" t="s">
+        <v>481</v>
+      </c>
+      <c r="C48" t="s">
+        <v>482</v>
+      </c>
+      <c r="D48" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" t="s">
+        <v>483</v>
+      </c>
+      <c r="F48" t="s">
+        <v>484</v>
+      </c>
+      <c r="G48" t="s">
+        <v>485</v>
+      </c>
+      <c r="J48" t="s">
+        <v>486</v>
+      </c>
+      <c r="K48" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48" t="s">
+        <v>487</v>
+      </c>
+      <c r="N48" t="s">
+        <v>488</v>
+      </c>
+      <c r="O48" t="s">
+        <v>489</v>
+      </c>
+      <c r="P48" t="s">
+        <v>490</v>
+      </c>
+      <c r="R48" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>124</v>
+      </c>
+      <c r="B49" t="s">
+        <v>492</v>
+      </c>
+      <c r="C49" t="s">
+        <v>493</v>
+      </c>
+      <c r="D49" t="s">
+        <v>259</v>
+      </c>
+      <c r="E49" t="s">
+        <v>494</v>
+      </c>
+      <c r="F49" t="s">
+        <v>495</v>
+      </c>
+      <c r="G49" t="s">
+        <v>48</v>
+      </c>
+      <c r="J49" t="s">
+        <v>496</v>
+      </c>
+      <c r="K49" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" t="s">
+        <v>27</v>
+      </c>
+      <c r="M49" t="s">
+        <v>497</v>
+      </c>
+      <c r="N49" t="s">
+        <v>498</v>
+      </c>
+      <c r="O49" t="s">
+        <v>499</v>
+      </c>
+      <c r="P49" t="s">
+        <v>500</v>
+      </c>
+      <c r="R49" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>125</v>
+      </c>
+      <c r="B50" t="s">
+        <v>501</v>
+      </c>
+      <c r="C50" t="s">
+        <v>502</v>
+      </c>
+      <c r="D50" t="s">
+        <v>503</v>
+      </c>
+      <c r="E50" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" t="s">
+        <v>504</v>
+      </c>
+      <c r="G50" t="s">
+        <v>48</v>
+      </c>
+      <c r="J50" t="s">
+        <v>505</v>
+      </c>
+      <c r="K50" t="s">
+        <v>26</v>
+      </c>
+      <c r="L50" t="s">
+        <v>27</v>
+      </c>
+      <c r="M50" t="s">
+        <v>506</v>
+      </c>
+      <c r="N50" t="s">
+        <v>507</v>
+      </c>
+      <c r="O50" t="s">
+        <v>508</v>
+      </c>
+      <c r="P50" t="s">
+        <v>509</v>
+      </c>
+      <c r="R50" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>127</v>
+      </c>
+      <c r="B51" t="s">
+        <v>510</v>
+      </c>
+      <c r="C51" t="s">
+        <v>511</v>
+      </c>
+      <c r="D51" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" t="s">
+        <v>512</v>
+      </c>
+      <c r="F51" t="s">
+        <v>513</v>
+      </c>
+      <c r="G51" t="s">
+        <v>218</v>
+      </c>
+      <c r="H51" t="s">
+        <v>514</v>
+      </c>
+      <c r="J51" t="s">
+        <v>24</v>
+      </c>
+      <c r="K51" t="s">
+        <v>132</v>
+      </c>
+      <c r="L51" t="s">
+        <v>27</v>
+      </c>
+      <c r="M51" t="s">
+        <v>515</v>
+      </c>
+      <c r="N51" t="s">
+        <v>516</v>
+      </c>
+      <c r="O51" t="s">
+        <v>517</v>
+      </c>
+      <c r="P51" t="s">
+        <v>518</v>
+      </c>
+      <c r="R51" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>128</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>519</v>
+      </c>
+      <c r="D52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" t="s">
+        <v>520</v>
+      </c>
+      <c r="F52" t="s">
+        <v>521</v>
+      </c>
+      <c r="G52" t="s">
+        <v>69</v>
+      </c>
+      <c r="J52" t="s">
+        <v>522</v>
+      </c>
+      <c r="K52" t="s">
+        <v>26</v>
+      </c>
+      <c r="L52" t="s">
+        <v>27</v>
+      </c>
+      <c r="M52" t="s">
+        <v>523</v>
+      </c>
+      <c r="N52" t="s">
+        <v>524</v>
+      </c>
+      <c r="O52" t="s">
+        <v>525</v>
+      </c>
+      <c r="P52" t="s">
+        <v>526</v>
+      </c>
+      <c r="R52" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>129</v>
+      </c>
+      <c r="B53" t="s">
+        <v>403</v>
+      </c>
+      <c r="C53" t="s">
+        <v>527</v>
+      </c>
+      <c r="D53" t="s">
+        <v>528</v>
+      </c>
+      <c r="E53" t="s">
+        <v>529</v>
+      </c>
+      <c r="F53" t="s">
+        <v>530</v>
+      </c>
+      <c r="G53" t="s">
+        <v>48</v>
+      </c>
+      <c r="J53" t="s">
+        <v>531</v>
+      </c>
+      <c r="K53" t="s">
+        <v>26</v>
+      </c>
+      <c r="L53" t="s">
+        <v>27</v>
+      </c>
+      <c r="M53" t="s">
+        <v>532</v>
+      </c>
+      <c r="N53" t="s">
+        <v>533</v>
+      </c>
+      <c r="O53" t="s">
+        <v>534</v>
+      </c>
+      <c r="P53" t="s">
+        <v>535</v>
+      </c>
+      <c r="R53" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>133</v>
+      </c>
+      <c r="B54" t="s">
+        <v>536</v>
+      </c>
+      <c r="C54" t="s">
+        <v>537</v>
+      </c>
+      <c r="D54" t="s">
+        <v>538</v>
+      </c>
+      <c r="E54" t="s">
+        <v>539</v>
+      </c>
+      <c r="F54" t="s">
+        <v>540</v>
+      </c>
+      <c r="G54" t="s">
+        <v>541</v>
+      </c>
+      <c r="J54" t="s">
+        <v>542</v>
+      </c>
+      <c r="K54" t="s">
+        <v>26</v>
+      </c>
+      <c r="L54" t="s">
+        <v>27</v>
+      </c>
+      <c r="M54" t="s">
+        <v>543</v>
+      </c>
+      <c r="N54" t="s">
+        <v>544</v>
+      </c>
+      <c r="O54" t="s">
+        <v>545</v>
+      </c>
+      <c r="P54" t="s">
+        <v>546</v>
+      </c>
+      <c r="R54" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
+        <v>547</v>
+      </c>
+      <c r="C55" t="s">
+        <v>548</v>
+      </c>
+      <c r="D55" t="s">
+        <v>549</v>
+      </c>
+      <c r="E55" t="s">
+        <v>550</v>
+      </c>
+      <c r="F55" t="s">
+        <v>551</v>
+      </c>
+      <c r="G55" t="s">
+        <v>552</v>
+      </c>
+      <c r="J55" t="s">
+        <v>553</v>
+      </c>
+      <c r="K55" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" t="s">
+        <v>27</v>
+      </c>
+      <c r="M55" t="s">
+        <v>554</v>
+      </c>
+      <c r="N55" t="s">
+        <v>555</v>
+      </c>
+      <c r="O55" t="s">
+        <v>556</v>
+      </c>
+      <c r="P55" t="s">
+        <v>557</v>
+      </c>
+      <c r="R55" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>136</v>
+      </c>
+      <c r="B56" t="s">
+        <v>558</v>
+      </c>
+      <c r="C56" t="s">
+        <v>559</v>
+      </c>
+      <c r="D56" t="s">
+        <v>560</v>
+      </c>
+      <c r="E56" t="s">
+        <v>561</v>
+      </c>
+      <c r="F56" t="s">
+        <v>562</v>
+      </c>
+      <c r="G56" t="s">
+        <v>563</v>
+      </c>
+      <c r="J56" t="s">
+        <v>564</v>
+      </c>
+      <c r="K56" t="s">
+        <v>26</v>
+      </c>
+      <c r="L56" t="s">
+        <v>27</v>
+      </c>
+      <c r="M56" t="s">
+        <v>565</v>
+      </c>
+      <c r="N56" t="s">
+        <v>566</v>
+      </c>
+      <c r="O56" t="s">
+        <v>567</v>
+      </c>
+      <c r="P56" t="s">
+        <v>568</v>
+      </c>
+      <c r="R56" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>137</v>
+      </c>
+      <c r="B57" t="s">
+        <v>411</v>
+      </c>
+      <c r="C57" t="s">
+        <v>570</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" t="s">
+        <v>571</v>
+      </c>
+      <c r="F57" t="s">
+        <v>572</v>
+      </c>
+      <c r="G57" t="s">
+        <v>218</v>
+      </c>
+      <c r="H57" t="s">
+        <v>131</v>
+      </c>
+      <c r="J57" t="s">
+        <v>24</v>
+      </c>
+      <c r="K57" t="s">
+        <v>132</v>
+      </c>
+      <c r="L57" t="s">
+        <v>27</v>
+      </c>
+      <c r="M57" t="s">
+        <v>573</v>
+      </c>
+      <c r="N57" t="s">
+        <v>574</v>
+      </c>
+      <c r="O57" t="s">
+        <v>575</v>
+      </c>
+      <c r="P57" t="s">
+        <v>576</v>
+      </c>
+      <c r="R57" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>141</v>
+      </c>
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" t="s">
+        <v>577</v>
+      </c>
+      <c r="D58" t="s">
+        <v>578</v>
+      </c>
+      <c r="E58" t="s">
+        <v>579</v>
+      </c>
+      <c r="F58" t="s">
+        <v>580</v>
+      </c>
+      <c r="G58" t="s">
+        <v>581</v>
+      </c>
+      <c r="J58" t="s">
+        <v>582</v>
+      </c>
+      <c r="K58" t="s">
+        <v>26</v>
+      </c>
+      <c r="L58" t="s">
+        <v>27</v>
+      </c>
+      <c r="M58" t="s">
+        <v>583</v>
+      </c>
+      <c r="N58" t="s">
+        <v>584</v>
+      </c>
+      <c r="O58" t="s">
+        <v>585</v>
+      </c>
+      <c r="P58" t="s">
+        <v>586</v>
+      </c>
+      <c r="R58" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>142</v>
+      </c>
+      <c r="B59" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" t="s">
+        <v>588</v>
+      </c>
+      <c r="D59" t="s">
+        <v>589</v>
+      </c>
+      <c r="E59" t="s">
+        <v>590</v>
+      </c>
+      <c r="F59" t="s">
+        <v>591</v>
+      </c>
+      <c r="G59" t="s">
+        <v>48</v>
+      </c>
+      <c r="J59" t="s">
+        <v>24</v>
+      </c>
+      <c r="K59" t="s">
+        <v>71</v>
+      </c>
+      <c r="L59" t="s">
+        <v>27</v>
+      </c>
+      <c r="M59" t="s">
+        <v>592</v>
+      </c>
+      <c r="N59" t="s">
+        <v>593</v>
+      </c>
+      <c r="O59" t="s">
+        <v>594</v>
+      </c>
+      <c r="P59" t="s">
+        <v>595</v>
+      </c>
+      <c r="R59" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>